<commit_message>
fixed except last req
</commit_message>
<xml_diff>
--- a/admin/templates/CASES.xlsx
+++ b/admin/templates/CASES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ex\devs\outbreak\admin\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5751FD-7DD3-4DA0-A959-52342216477D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02ACC64-EA05-4279-82A4-2EB7D8CCFA05}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1538,6 +1538,42 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1565,47 +1601,17 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1639,12 +1645,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2305,8 +2305,8 @@
   </sheetPr>
   <dimension ref="A1:BF62"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="M22" zoomScale="85" zoomScaleNormal="106" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="BD10" sqref="BD10:BD34"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="M1" zoomScale="85" zoomScaleNormal="106" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="AL12" sqref="AL12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2331,307 +2331,307 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" s="29" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="159" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="147"/>
-      <c r="G1" s="147"/>
-      <c r="H1" s="147"/>
-      <c r="I1" s="147"/>
-      <c r="J1" s="147"/>
-      <c r="K1" s="147"/>
-      <c r="L1" s="147"/>
-      <c r="M1" s="147"/>
-      <c r="N1" s="147"/>
-      <c r="O1" s="147"/>
-      <c r="P1" s="147"/>
-      <c r="Q1" s="147"/>
-      <c r="R1" s="147"/>
-      <c r="S1" s="147"/>
-      <c r="T1" s="147"/>
-      <c r="U1" s="147"/>
-      <c r="V1" s="147"/>
-      <c r="W1" s="147"/>
-      <c r="X1" s="147"/>
-      <c r="Y1" s="147"/>
-      <c r="Z1" s="147"/>
-      <c r="AA1" s="147"/>
-      <c r="AB1" s="147"/>
-      <c r="AC1" s="147"/>
-      <c r="AD1" s="147"/>
-      <c r="AE1" s="147"/>
-      <c r="AF1" s="147"/>
-      <c r="AG1" s="147"/>
-      <c r="AH1" s="147"/>
-      <c r="AI1" s="147"/>
-      <c r="AJ1" s="147"/>
-      <c r="AK1" s="147"/>
-      <c r="AL1" s="147"/>
-      <c r="AM1" s="147"/>
-      <c r="AN1" s="147"/>
-      <c r="AO1" s="147"/>
-      <c r="AP1" s="147"/>
-      <c r="AQ1" s="147"/>
-      <c r="AR1" s="147"/>
-      <c r="AS1" s="147"/>
-      <c r="AT1" s="147"/>
-      <c r="AU1" s="147"/>
-      <c r="AV1" s="147"/>
-      <c r="AW1" s="147"/>
-      <c r="AX1" s="147"/>
-      <c r="AY1" s="147"/>
-      <c r="AZ1" s="147"/>
-      <c r="BA1" s="147"/>
-      <c r="BB1" s="147"/>
-      <c r="BC1" s="147"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="159"/>
+      <c r="E1" s="159"/>
+      <c r="F1" s="159"/>
+      <c r="G1" s="159"/>
+      <c r="H1" s="159"/>
+      <c r="I1" s="159"/>
+      <c r="J1" s="159"/>
+      <c r="K1" s="159"/>
+      <c r="L1" s="159"/>
+      <c r="M1" s="159"/>
+      <c r="N1" s="159"/>
+      <c r="O1" s="159"/>
+      <c r="P1" s="159"/>
+      <c r="Q1" s="159"/>
+      <c r="R1" s="159"/>
+      <c r="S1" s="159"/>
+      <c r="T1" s="159"/>
+      <c r="U1" s="159"/>
+      <c r="V1" s="159"/>
+      <c r="W1" s="159"/>
+      <c r="X1" s="159"/>
+      <c r="Y1" s="159"/>
+      <c r="Z1" s="159"/>
+      <c r="AA1" s="159"/>
+      <c r="AB1" s="159"/>
+      <c r="AC1" s="159"/>
+      <c r="AD1" s="159"/>
+      <c r="AE1" s="159"/>
+      <c r="AF1" s="159"/>
+      <c r="AG1" s="159"/>
+      <c r="AH1" s="159"/>
+      <c r="AI1" s="159"/>
+      <c r="AJ1" s="159"/>
+      <c r="AK1" s="159"/>
+      <c r="AL1" s="159"/>
+      <c r="AM1" s="159"/>
+      <c r="AN1" s="159"/>
+      <c r="AO1" s="159"/>
+      <c r="AP1" s="159"/>
+      <c r="AQ1" s="159"/>
+      <c r="AR1" s="159"/>
+      <c r="AS1" s="159"/>
+      <c r="AT1" s="159"/>
+      <c r="AU1" s="159"/>
+      <c r="AV1" s="159"/>
+      <c r="AW1" s="159"/>
+      <c r="AX1" s="159"/>
+      <c r="AY1" s="159"/>
+      <c r="AZ1" s="159"/>
+      <c r="BA1" s="159"/>
+      <c r="BB1" s="159"/>
+      <c r="BC1" s="159"/>
       <c r="BD1" s="28"/>
       <c r="BF1" s="30"/>
     </row>
     <row r="2" spans="1:58" s="29" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="147" t="s">
+      <c r="A2" s="159" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="147"/>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
-      <c r="E2" s="147"/>
-      <c r="F2" s="147"/>
-      <c r="G2" s="147"/>
-      <c r="H2" s="147"/>
-      <c r="I2" s="147"/>
-      <c r="J2" s="147"/>
-      <c r="K2" s="147"/>
-      <c r="L2" s="147"/>
-      <c r="M2" s="147"/>
-      <c r="N2" s="147"/>
-      <c r="O2" s="147"/>
-      <c r="P2" s="147"/>
-      <c r="Q2" s="147"/>
-      <c r="R2" s="147"/>
-      <c r="S2" s="147"/>
-      <c r="T2" s="147"/>
-      <c r="U2" s="147"/>
-      <c r="V2" s="147"/>
-      <c r="W2" s="147"/>
-      <c r="X2" s="147"/>
-      <c r="Y2" s="147"/>
-      <c r="Z2" s="147"/>
-      <c r="AA2" s="147"/>
-      <c r="AB2" s="147"/>
-      <c r="AC2" s="147"/>
-      <c r="AD2" s="147"/>
-      <c r="AE2" s="147"/>
-      <c r="AF2" s="147"/>
-      <c r="AG2" s="147"/>
-      <c r="AH2" s="147"/>
-      <c r="AI2" s="147"/>
-      <c r="AJ2" s="147"/>
-      <c r="AK2" s="147"/>
-      <c r="AL2" s="147"/>
-      <c r="AM2" s="147"/>
-      <c r="AN2" s="147"/>
-      <c r="AO2" s="147"/>
-      <c r="AP2" s="147"/>
-      <c r="AQ2" s="147"/>
-      <c r="AR2" s="147"/>
-      <c r="AS2" s="147"/>
-      <c r="AT2" s="147"/>
-      <c r="AU2" s="147"/>
-      <c r="AV2" s="147"/>
-      <c r="AW2" s="147"/>
-      <c r="AX2" s="147"/>
-      <c r="AY2" s="147"/>
-      <c r="AZ2" s="147"/>
-      <c r="BA2" s="147"/>
-      <c r="BB2" s="147"/>
-      <c r="BC2" s="147"/>
+      <c r="B2" s="159"/>
+      <c r="C2" s="159"/>
+      <c r="D2" s="159"/>
+      <c r="E2" s="159"/>
+      <c r="F2" s="159"/>
+      <c r="G2" s="159"/>
+      <c r="H2" s="159"/>
+      <c r="I2" s="159"/>
+      <c r="J2" s="159"/>
+      <c r="K2" s="159"/>
+      <c r="L2" s="159"/>
+      <c r="M2" s="159"/>
+      <c r="N2" s="159"/>
+      <c r="O2" s="159"/>
+      <c r="P2" s="159"/>
+      <c r="Q2" s="159"/>
+      <c r="R2" s="159"/>
+      <c r="S2" s="159"/>
+      <c r="T2" s="159"/>
+      <c r="U2" s="159"/>
+      <c r="V2" s="159"/>
+      <c r="W2" s="159"/>
+      <c r="X2" s="159"/>
+      <c r="Y2" s="159"/>
+      <c r="Z2" s="159"/>
+      <c r="AA2" s="159"/>
+      <c r="AB2" s="159"/>
+      <c r="AC2" s="159"/>
+      <c r="AD2" s="159"/>
+      <c r="AE2" s="159"/>
+      <c r="AF2" s="159"/>
+      <c r="AG2" s="159"/>
+      <c r="AH2" s="159"/>
+      <c r="AI2" s="159"/>
+      <c r="AJ2" s="159"/>
+      <c r="AK2" s="159"/>
+      <c r="AL2" s="159"/>
+      <c r="AM2" s="159"/>
+      <c r="AN2" s="159"/>
+      <c r="AO2" s="159"/>
+      <c r="AP2" s="159"/>
+      <c r="AQ2" s="159"/>
+      <c r="AR2" s="159"/>
+      <c r="AS2" s="159"/>
+      <c r="AT2" s="159"/>
+      <c r="AU2" s="159"/>
+      <c r="AV2" s="159"/>
+      <c r="AW2" s="159"/>
+      <c r="AX2" s="159"/>
+      <c r="AY2" s="159"/>
+      <c r="AZ2" s="159"/>
+      <c r="BA2" s="159"/>
+      <c r="BB2" s="159"/>
+      <c r="BC2" s="159"/>
       <c r="BD2" s="28"/>
       <c r="BF2" s="30"/>
     </row>
     <row r="3" spans="1:58" s="29" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="148" t="s">
+      <c r="A3" s="160" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="148"/>
-      <c r="C3" s="148"/>
-      <c r="D3" s="148"/>
-      <c r="E3" s="148"/>
-      <c r="F3" s="148"/>
-      <c r="G3" s="148"/>
-      <c r="H3" s="148"/>
-      <c r="I3" s="148"/>
-      <c r="J3" s="148"/>
-      <c r="K3" s="148"/>
-      <c r="L3" s="148"/>
-      <c r="M3" s="148"/>
-      <c r="N3" s="148"/>
-      <c r="O3" s="148"/>
-      <c r="P3" s="148"/>
-      <c r="Q3" s="148"/>
-      <c r="R3" s="148"/>
-      <c r="S3" s="148"/>
-      <c r="T3" s="148"/>
-      <c r="U3" s="148"/>
-      <c r="V3" s="148"/>
-      <c r="W3" s="148"/>
-      <c r="X3" s="148"/>
-      <c r="Y3" s="148"/>
-      <c r="Z3" s="148"/>
-      <c r="AA3" s="148"/>
-      <c r="AB3" s="148"/>
-      <c r="AC3" s="148"/>
-      <c r="AD3" s="148"/>
-      <c r="AE3" s="148"/>
-      <c r="AF3" s="148"/>
-      <c r="AG3" s="148"/>
-      <c r="AH3" s="148"/>
-      <c r="AI3" s="148"/>
-      <c r="AJ3" s="148"/>
-      <c r="AK3" s="148"/>
-      <c r="AL3" s="148"/>
-      <c r="AM3" s="148"/>
-      <c r="AN3" s="148"/>
-      <c r="AO3" s="148"/>
-      <c r="AP3" s="148"/>
-      <c r="AQ3" s="148"/>
-      <c r="AR3" s="148"/>
-      <c r="AS3" s="148"/>
-      <c r="AT3" s="148"/>
-      <c r="AU3" s="148"/>
-      <c r="AV3" s="148"/>
-      <c r="AW3" s="148"/>
-      <c r="AX3" s="148"/>
-      <c r="AY3" s="148"/>
-      <c r="AZ3" s="148"/>
-      <c r="BA3" s="148"/>
-      <c r="BB3" s="148"/>
-      <c r="BC3" s="148"/>
+      <c r="B3" s="160"/>
+      <c r="C3" s="160"/>
+      <c r="D3" s="160"/>
+      <c r="E3" s="160"/>
+      <c r="F3" s="160"/>
+      <c r="G3" s="160"/>
+      <c r="H3" s="160"/>
+      <c r="I3" s="160"/>
+      <c r="J3" s="160"/>
+      <c r="K3" s="160"/>
+      <c r="L3" s="160"/>
+      <c r="M3" s="160"/>
+      <c r="N3" s="160"/>
+      <c r="O3" s="160"/>
+      <c r="P3" s="160"/>
+      <c r="Q3" s="160"/>
+      <c r="R3" s="160"/>
+      <c r="S3" s="160"/>
+      <c r="T3" s="160"/>
+      <c r="U3" s="160"/>
+      <c r="V3" s="160"/>
+      <c r="W3" s="160"/>
+      <c r="X3" s="160"/>
+      <c r="Y3" s="160"/>
+      <c r="Z3" s="160"/>
+      <c r="AA3" s="160"/>
+      <c r="AB3" s="160"/>
+      <c r="AC3" s="160"/>
+      <c r="AD3" s="160"/>
+      <c r="AE3" s="160"/>
+      <c r="AF3" s="160"/>
+      <c r="AG3" s="160"/>
+      <c r="AH3" s="160"/>
+      <c r="AI3" s="160"/>
+      <c r="AJ3" s="160"/>
+      <c r="AK3" s="160"/>
+      <c r="AL3" s="160"/>
+      <c r="AM3" s="160"/>
+      <c r="AN3" s="160"/>
+      <c r="AO3" s="160"/>
+      <c r="AP3" s="160"/>
+      <c r="AQ3" s="160"/>
+      <c r="AR3" s="160"/>
+      <c r="AS3" s="160"/>
+      <c r="AT3" s="160"/>
+      <c r="AU3" s="160"/>
+      <c r="AV3" s="160"/>
+      <c r="AW3" s="160"/>
+      <c r="AX3" s="160"/>
+      <c r="AY3" s="160"/>
+      <c r="AZ3" s="160"/>
+      <c r="BA3" s="160"/>
+      <c r="BB3" s="160"/>
+      <c r="BC3" s="160"/>
       <c r="BD3" s="28"/>
       <c r="BF3" s="30"/>
     </row>
     <row r="4" spans="1:58" s="29" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="147" t="s">
+      <c r="A4" s="159" t="s">
         <v>142</v>
       </c>
-      <c r="B4" s="147"/>
-      <c r="C4" s="147"/>
-      <c r="D4" s="147"/>
-      <c r="E4" s="147"/>
-      <c r="F4" s="147"/>
-      <c r="G4" s="147"/>
-      <c r="H4" s="147"/>
-      <c r="I4" s="147"/>
-      <c r="J4" s="147"/>
-      <c r="K4" s="147"/>
-      <c r="L4" s="147"/>
-      <c r="M4" s="147"/>
-      <c r="N4" s="147"/>
-      <c r="O4" s="147"/>
-      <c r="P4" s="147"/>
-      <c r="Q4" s="147"/>
-      <c r="R4" s="147"/>
-      <c r="S4" s="147"/>
-      <c r="T4" s="147"/>
-      <c r="U4" s="147"/>
-      <c r="V4" s="147"/>
-      <c r="W4" s="147"/>
-      <c r="X4" s="147"/>
-      <c r="Y4" s="147"/>
-      <c r="Z4" s="147"/>
-      <c r="AA4" s="147"/>
-      <c r="AB4" s="147"/>
-      <c r="AC4" s="147"/>
-      <c r="AD4" s="147"/>
-      <c r="AE4" s="147"/>
-      <c r="AF4" s="147"/>
-      <c r="AG4" s="147"/>
-      <c r="AH4" s="147"/>
-      <c r="AI4" s="147"/>
-      <c r="AJ4" s="147"/>
-      <c r="AK4" s="147"/>
-      <c r="AL4" s="147"/>
-      <c r="AM4" s="147"/>
-      <c r="AN4" s="147"/>
-      <c r="AO4" s="147"/>
-      <c r="AP4" s="147"/>
-      <c r="AQ4" s="147"/>
-      <c r="AR4" s="147"/>
-      <c r="AS4" s="147"/>
-      <c r="AT4" s="147"/>
-      <c r="AU4" s="147"/>
-      <c r="AV4" s="147"/>
-      <c r="AW4" s="147"/>
-      <c r="AX4" s="147"/>
-      <c r="AY4" s="147"/>
-      <c r="AZ4" s="147"/>
-      <c r="BA4" s="147"/>
-      <c r="BB4" s="147"/>
-      <c r="BC4" s="147"/>
+      <c r="B4" s="159"/>
+      <c r="C4" s="159"/>
+      <c r="D4" s="159"/>
+      <c r="E4" s="159"/>
+      <c r="F4" s="159"/>
+      <c r="G4" s="159"/>
+      <c r="H4" s="159"/>
+      <c r="I4" s="159"/>
+      <c r="J4" s="159"/>
+      <c r="K4" s="159"/>
+      <c r="L4" s="159"/>
+      <c r="M4" s="159"/>
+      <c r="N4" s="159"/>
+      <c r="O4" s="159"/>
+      <c r="P4" s="159"/>
+      <c r="Q4" s="159"/>
+      <c r="R4" s="159"/>
+      <c r="S4" s="159"/>
+      <c r="T4" s="159"/>
+      <c r="U4" s="159"/>
+      <c r="V4" s="159"/>
+      <c r="W4" s="159"/>
+      <c r="X4" s="159"/>
+      <c r="Y4" s="159"/>
+      <c r="Z4" s="159"/>
+      <c r="AA4" s="159"/>
+      <c r="AB4" s="159"/>
+      <c r="AC4" s="159"/>
+      <c r="AD4" s="159"/>
+      <c r="AE4" s="159"/>
+      <c r="AF4" s="159"/>
+      <c r="AG4" s="159"/>
+      <c r="AH4" s="159"/>
+      <c r="AI4" s="159"/>
+      <c r="AJ4" s="159"/>
+      <c r="AK4" s="159"/>
+      <c r="AL4" s="159"/>
+      <c r="AM4" s="159"/>
+      <c r="AN4" s="159"/>
+      <c r="AO4" s="159"/>
+      <c r="AP4" s="159"/>
+      <c r="AQ4" s="159"/>
+      <c r="AR4" s="159"/>
+      <c r="AS4" s="159"/>
+      <c r="AT4" s="159"/>
+      <c r="AU4" s="159"/>
+      <c r="AV4" s="159"/>
+      <c r="AW4" s="159"/>
+      <c r="AX4" s="159"/>
+      <c r="AY4" s="159"/>
+      <c r="AZ4" s="159"/>
+      <c r="BA4" s="159"/>
+      <c r="BB4" s="159"/>
+      <c r="BC4" s="159"/>
       <c r="BD4" s="28"/>
       <c r="BF4" s="30"/>
     </row>
     <row r="5" spans="1:58" s="29" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="149" t="s">
+      <c r="A5" s="161" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="149"/>
-      <c r="C5" s="149"/>
-      <c r="D5" s="149"/>
-      <c r="E5" s="149"/>
-      <c r="F5" s="149"/>
-      <c r="G5" s="149"/>
-      <c r="H5" s="149"/>
-      <c r="I5" s="149"/>
-      <c r="J5" s="149"/>
-      <c r="K5" s="149"/>
-      <c r="L5" s="149"/>
-      <c r="M5" s="149"/>
-      <c r="N5" s="149"/>
-      <c r="O5" s="149"/>
-      <c r="P5" s="149"/>
-      <c r="Q5" s="149"/>
-      <c r="R5" s="149"/>
-      <c r="S5" s="149"/>
-      <c r="T5" s="149"/>
-      <c r="U5" s="149"/>
-      <c r="V5" s="149"/>
-      <c r="W5" s="149"/>
-      <c r="X5" s="149"/>
-      <c r="Y5" s="149"/>
-      <c r="Z5" s="149"/>
-      <c r="AA5" s="149"/>
-      <c r="AB5" s="149"/>
-      <c r="AC5" s="149"/>
-      <c r="AD5" s="149"/>
-      <c r="AE5" s="149"/>
-      <c r="AF5" s="149"/>
-      <c r="AG5" s="149"/>
-      <c r="AH5" s="149"/>
-      <c r="AI5" s="149"/>
-      <c r="AJ5" s="149"/>
-      <c r="AK5" s="149"/>
-      <c r="AL5" s="149"/>
-      <c r="AM5" s="149"/>
-      <c r="AN5" s="149"/>
-      <c r="AO5" s="149"/>
-      <c r="AP5" s="149"/>
-      <c r="AQ5" s="149"/>
-      <c r="AR5" s="149"/>
-      <c r="AS5" s="149"/>
-      <c r="AT5" s="149"/>
-      <c r="AU5" s="149"/>
-      <c r="AV5" s="149"/>
-      <c r="AW5" s="149"/>
-      <c r="AX5" s="149"/>
-      <c r="AY5" s="149"/>
-      <c r="AZ5" s="149"/>
-      <c r="BA5" s="149"/>
-      <c r="BB5" s="149"/>
-      <c r="BC5" s="149"/>
+      <c r="B5" s="161"/>
+      <c r="C5" s="161"/>
+      <c r="D5" s="161"/>
+      <c r="E5" s="161"/>
+      <c r="F5" s="161"/>
+      <c r="G5" s="161"/>
+      <c r="H5" s="161"/>
+      <c r="I5" s="161"/>
+      <c r="J5" s="161"/>
+      <c r="K5" s="161"/>
+      <c r="L5" s="161"/>
+      <c r="M5" s="161"/>
+      <c r="N5" s="161"/>
+      <c r="O5" s="161"/>
+      <c r="P5" s="161"/>
+      <c r="Q5" s="161"/>
+      <c r="R5" s="161"/>
+      <c r="S5" s="161"/>
+      <c r="T5" s="161"/>
+      <c r="U5" s="161"/>
+      <c r="V5" s="161"/>
+      <c r="W5" s="161"/>
+      <c r="X5" s="161"/>
+      <c r="Y5" s="161"/>
+      <c r="Z5" s="161"/>
+      <c r="AA5" s="161"/>
+      <c r="AB5" s="161"/>
+      <c r="AC5" s="161"/>
+      <c r="AD5" s="161"/>
+      <c r="AE5" s="161"/>
+      <c r="AF5" s="161"/>
+      <c r="AG5" s="161"/>
+      <c r="AH5" s="161"/>
+      <c r="AI5" s="161"/>
+      <c r="AJ5" s="161"/>
+      <c r="AK5" s="161"/>
+      <c r="AL5" s="161"/>
+      <c r="AM5" s="161"/>
+      <c r="AN5" s="161"/>
+      <c r="AO5" s="161"/>
+      <c r="AP5" s="161"/>
+      <c r="AQ5" s="161"/>
+      <c r="AR5" s="161"/>
+      <c r="AS5" s="161"/>
+      <c r="AT5" s="161"/>
+      <c r="AU5" s="161"/>
+      <c r="AV5" s="161"/>
+      <c r="AW5" s="161"/>
+      <c r="AX5" s="161"/>
+      <c r="AY5" s="161"/>
+      <c r="AZ5" s="161"/>
+      <c r="BA5" s="161"/>
+      <c r="BB5" s="161"/>
+      <c r="BC5" s="161"/>
       <c r="BD5" s="28"/>
       <c r="BF5" s="30"/>
     </row>
@@ -2695,95 +2695,95 @@
       <c r="BF6" s="30"/>
     </row>
     <row r="7" spans="1:58" s="29" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="160" t="s">
+      <c r="A7" s="149" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="161"/>
-      <c r="C7" s="144" t="s">
+      <c r="B7" s="150"/>
+      <c r="C7" s="156" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="145"/>
-      <c r="E7" s="145"/>
-      <c r="F7" s="145"/>
-      <c r="G7" s="145"/>
-      <c r="H7" s="146"/>
-      <c r="I7" s="157" t="s">
+      <c r="D7" s="157"/>
+      <c r="E7" s="157"/>
+      <c r="F7" s="157"/>
+      <c r="G7" s="157"/>
+      <c r="H7" s="158"/>
+      <c r="I7" s="143" t="s">
         <v>64</v>
       </c>
-      <c r="J7" s="158"/>
-      <c r="K7" s="158"/>
-      <c r="L7" s="159"/>
-      <c r="M7" s="150" t="s">
+      <c r="J7" s="144"/>
+      <c r="K7" s="144"/>
+      <c r="L7" s="145"/>
+      <c r="M7" s="146" t="s">
         <v>65</v>
       </c>
-      <c r="N7" s="151"/>
-      <c r="O7" s="151"/>
-      <c r="P7" s="151"/>
-      <c r="Q7" s="152"/>
-      <c r="R7" s="150" t="s">
+      <c r="N7" s="147"/>
+      <c r="O7" s="147"/>
+      <c r="P7" s="147"/>
+      <c r="Q7" s="148"/>
+      <c r="R7" s="146" t="s">
         <v>66</v>
       </c>
-      <c r="S7" s="151"/>
-      <c r="T7" s="151"/>
-      <c r="U7" s="152"/>
-      <c r="V7" s="157" t="s">
+      <c r="S7" s="147"/>
+      <c r="T7" s="147"/>
+      <c r="U7" s="148"/>
+      <c r="V7" s="143" t="s">
         <v>55</v>
       </c>
-      <c r="W7" s="158"/>
-      <c r="X7" s="158"/>
-      <c r="Y7" s="159"/>
-      <c r="Z7" s="150" t="s">
+      <c r="W7" s="144"/>
+      <c r="X7" s="144"/>
+      <c r="Y7" s="145"/>
+      <c r="Z7" s="146" t="s">
         <v>56</v>
       </c>
-      <c r="AA7" s="151"/>
-      <c r="AB7" s="151"/>
-      <c r="AC7" s="151"/>
-      <c r="AD7" s="152"/>
-      <c r="AE7" s="150" t="s">
+      <c r="AA7" s="147"/>
+      <c r="AB7" s="147"/>
+      <c r="AC7" s="147"/>
+      <c r="AD7" s="148"/>
+      <c r="AE7" s="146" t="s">
         <v>57</v>
       </c>
-      <c r="AF7" s="151"/>
-      <c r="AG7" s="151"/>
-      <c r="AH7" s="152"/>
-      <c r="AI7" s="150" t="s">
+      <c r="AF7" s="147"/>
+      <c r="AG7" s="147"/>
+      <c r="AH7" s="148"/>
+      <c r="AI7" s="146" t="s">
         <v>58</v>
       </c>
-      <c r="AJ7" s="151"/>
-      <c r="AK7" s="151"/>
-      <c r="AL7" s="151"/>
-      <c r="AM7" s="152"/>
-      <c r="AN7" s="150" t="s">
+      <c r="AJ7" s="147"/>
+      <c r="AK7" s="147"/>
+      <c r="AL7" s="147"/>
+      <c r="AM7" s="148"/>
+      <c r="AN7" s="146" t="s">
         <v>59</v>
       </c>
-      <c r="AO7" s="151"/>
-      <c r="AP7" s="151"/>
-      <c r="AQ7" s="152"/>
-      <c r="AR7" s="157" t="s">
+      <c r="AO7" s="147"/>
+      <c r="AP7" s="147"/>
+      <c r="AQ7" s="148"/>
+      <c r="AR7" s="143" t="s">
         <v>60</v>
       </c>
-      <c r="AS7" s="158"/>
-      <c r="AT7" s="158"/>
-      <c r="AU7" s="159"/>
-      <c r="AV7" s="150" t="s">
+      <c r="AS7" s="144"/>
+      <c r="AT7" s="144"/>
+      <c r="AU7" s="145"/>
+      <c r="AV7" s="146" t="s">
         <v>61</v>
       </c>
-      <c r="AW7" s="151"/>
-      <c r="AX7" s="151"/>
-      <c r="AY7" s="152"/>
-      <c r="AZ7" s="150" t="s">
+      <c r="AW7" s="147"/>
+      <c r="AX7" s="147"/>
+      <c r="AY7" s="148"/>
+      <c r="AZ7" s="146" t="s">
         <v>62</v>
       </c>
-      <c r="BA7" s="151"/>
-      <c r="BB7" s="151"/>
-      <c r="BC7" s="152"/>
-      <c r="BD7" s="141" t="s">
+      <c r="BA7" s="147"/>
+      <c r="BB7" s="147"/>
+      <c r="BC7" s="148"/>
+      <c r="BD7" s="153" t="s">
         <v>96</v>
       </c>
       <c r="BF7" s="30"/>
     </row>
     <row r="8" spans="1:58" s="29" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="162"/>
-      <c r="B8" s="163"/>
+      <c r="A8" s="151"/>
+      <c r="B8" s="152"/>
       <c r="C8" s="34"/>
       <c r="D8" s="33"/>
       <c r="E8" s="34"/>
@@ -2837,14 +2837,14 @@
       <c r="BA8" s="36"/>
       <c r="BB8" s="36"/>
       <c r="BC8" s="37"/>
-      <c r="BD8" s="142"/>
+      <c r="BD8" s="154"/>
       <c r="BF8" s="30"/>
     </row>
     <row r="9" spans="1:58" s="29" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="153" t="s">
+      <c r="A9" s="162" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="154"/>
+      <c r="B9" s="163"/>
       <c r="C9" s="137" t="s">
         <v>143</v>
       </c>
@@ -3004,7 +3004,7 @@
       <c r="BC9" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="BD9" s="143"/>
+      <c r="BD9" s="155"/>
       <c r="BF9" s="30"/>
     </row>
     <row r="10" spans="1:58" s="29" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4561,10 +4561,10 @@
       <c r="BF34" s="30"/>
     </row>
     <row r="35" spans="1:58" s="29" customFormat="1" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="155" t="s">
+      <c r="A35" s="141" t="s">
         <v>95</v>
       </c>
-      <c r="B35" s="156"/>
+      <c r="B35" s="142"/>
       <c r="C35" s="70">
         <f t="shared" ref="C35:BC35" si="1">SUM(C10:C34)</f>
         <v>0</v>
@@ -4908,15 +4908,6 @@
     <sortCondition ref="B37"/>
   </sortState>
   <mergeCells count="21">
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="V7:Y7"/>
-    <mergeCell ref="Z7:AD7"/>
-    <mergeCell ref="AE7:AH7"/>
-    <mergeCell ref="AI7:AM7"/>
-    <mergeCell ref="A7:B8"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="M7:Q7"/>
-    <mergeCell ref="R7:U7"/>
     <mergeCell ref="BD7:BD9"/>
     <mergeCell ref="C7:H7"/>
     <mergeCell ref="A1:BC1"/>
@@ -4929,9 +4920,18 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="AN7:AQ7"/>
     <mergeCell ref="AR7:AU7"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="V7:Y7"/>
+    <mergeCell ref="Z7:AD7"/>
+    <mergeCell ref="AE7:AH7"/>
+    <mergeCell ref="AI7:AM7"/>
+    <mergeCell ref="A7:B8"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="M7:Q7"/>
+    <mergeCell ref="R7:U7"/>
   </mergeCells>
   <pageMargins left="0.25" right="1.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" scale="52" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="5" scale="53" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -4968,302 +4968,302 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:57" s="29" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="159" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="147"/>
-      <c r="G1" s="147"/>
-      <c r="H1" s="147"/>
-      <c r="I1" s="147"/>
-      <c r="J1" s="147"/>
-      <c r="K1" s="147"/>
-      <c r="L1" s="147"/>
-      <c r="M1" s="147"/>
-      <c r="N1" s="147"/>
-      <c r="O1" s="147"/>
-      <c r="P1" s="147"/>
-      <c r="Q1" s="147"/>
-      <c r="R1" s="147"/>
-      <c r="S1" s="147"/>
-      <c r="T1" s="147"/>
-      <c r="U1" s="147"/>
-      <c r="V1" s="147"/>
-      <c r="W1" s="147"/>
-      <c r="X1" s="147"/>
-      <c r="Y1" s="147"/>
-      <c r="Z1" s="147"/>
-      <c r="AA1" s="147"/>
-      <c r="AB1" s="147"/>
-      <c r="AC1" s="147"/>
-      <c r="AD1" s="147"/>
-      <c r="AE1" s="147"/>
-      <c r="AF1" s="147"/>
-      <c r="AG1" s="147"/>
-      <c r="AH1" s="147"/>
-      <c r="AI1" s="147"/>
-      <c r="AJ1" s="147"/>
-      <c r="AK1" s="147"/>
-      <c r="AL1" s="147"/>
-      <c r="AM1" s="147"/>
-      <c r="AN1" s="147"/>
-      <c r="AO1" s="147"/>
-      <c r="AP1" s="147"/>
-      <c r="AQ1" s="147"/>
-      <c r="AR1" s="147"/>
-      <c r="AS1" s="147"/>
-      <c r="AT1" s="147"/>
-      <c r="AU1" s="147"/>
-      <c r="AV1" s="147"/>
-      <c r="AW1" s="147"/>
-      <c r="AX1" s="147"/>
-      <c r="AY1" s="147"/>
-      <c r="AZ1" s="147"/>
-      <c r="BA1" s="147"/>
-      <c r="BB1" s="147"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="159"/>
+      <c r="E1" s="159"/>
+      <c r="F1" s="159"/>
+      <c r="G1" s="159"/>
+      <c r="H1" s="159"/>
+      <c r="I1" s="159"/>
+      <c r="J1" s="159"/>
+      <c r="K1" s="159"/>
+      <c r="L1" s="159"/>
+      <c r="M1" s="159"/>
+      <c r="N1" s="159"/>
+      <c r="O1" s="159"/>
+      <c r="P1" s="159"/>
+      <c r="Q1" s="159"/>
+      <c r="R1" s="159"/>
+      <c r="S1" s="159"/>
+      <c r="T1" s="159"/>
+      <c r="U1" s="159"/>
+      <c r="V1" s="159"/>
+      <c r="W1" s="159"/>
+      <c r="X1" s="159"/>
+      <c r="Y1" s="159"/>
+      <c r="Z1" s="159"/>
+      <c r="AA1" s="159"/>
+      <c r="AB1" s="159"/>
+      <c r="AC1" s="159"/>
+      <c r="AD1" s="159"/>
+      <c r="AE1" s="159"/>
+      <c r="AF1" s="159"/>
+      <c r="AG1" s="159"/>
+      <c r="AH1" s="159"/>
+      <c r="AI1" s="159"/>
+      <c r="AJ1" s="159"/>
+      <c r="AK1" s="159"/>
+      <c r="AL1" s="159"/>
+      <c r="AM1" s="159"/>
+      <c r="AN1" s="159"/>
+      <c r="AO1" s="159"/>
+      <c r="AP1" s="159"/>
+      <c r="AQ1" s="159"/>
+      <c r="AR1" s="159"/>
+      <c r="AS1" s="159"/>
+      <c r="AT1" s="159"/>
+      <c r="AU1" s="159"/>
+      <c r="AV1" s="159"/>
+      <c r="AW1" s="159"/>
+      <c r="AX1" s="159"/>
+      <c r="AY1" s="159"/>
+      <c r="AZ1" s="159"/>
+      <c r="BA1" s="159"/>
+      <c r="BB1" s="159"/>
       <c r="BC1" s="96"/>
       <c r="BE1" s="30"/>
     </row>
     <row r="2" spans="1:57" s="29" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="147" t="s">
+      <c r="A2" s="159" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="147"/>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
-      <c r="E2" s="147"/>
-      <c r="F2" s="147"/>
-      <c r="G2" s="147"/>
-      <c r="H2" s="147"/>
-      <c r="I2" s="147"/>
-      <c r="J2" s="147"/>
-      <c r="K2" s="147"/>
-      <c r="L2" s="147"/>
-      <c r="M2" s="147"/>
-      <c r="N2" s="147"/>
-      <c r="O2" s="147"/>
-      <c r="P2" s="147"/>
-      <c r="Q2" s="147"/>
-      <c r="R2" s="147"/>
-      <c r="S2" s="147"/>
-      <c r="T2" s="147"/>
-      <c r="U2" s="147"/>
-      <c r="V2" s="147"/>
-      <c r="W2" s="147"/>
-      <c r="X2" s="147"/>
-      <c r="Y2" s="147"/>
-      <c r="Z2" s="147"/>
-      <c r="AA2" s="147"/>
-      <c r="AB2" s="147"/>
-      <c r="AC2" s="147"/>
-      <c r="AD2" s="147"/>
-      <c r="AE2" s="147"/>
-      <c r="AF2" s="147"/>
-      <c r="AG2" s="147"/>
-      <c r="AH2" s="147"/>
-      <c r="AI2" s="147"/>
-      <c r="AJ2" s="147"/>
-      <c r="AK2" s="147"/>
-      <c r="AL2" s="147"/>
-      <c r="AM2" s="147"/>
-      <c r="AN2" s="147"/>
-      <c r="AO2" s="147"/>
-      <c r="AP2" s="147"/>
-      <c r="AQ2" s="147"/>
-      <c r="AR2" s="147"/>
-      <c r="AS2" s="147"/>
-      <c r="AT2" s="147"/>
-      <c r="AU2" s="147"/>
-      <c r="AV2" s="147"/>
-      <c r="AW2" s="147"/>
-      <c r="AX2" s="147"/>
-      <c r="AY2" s="147"/>
-      <c r="AZ2" s="147"/>
-      <c r="BA2" s="147"/>
-      <c r="BB2" s="147"/>
+      <c r="B2" s="159"/>
+      <c r="C2" s="159"/>
+      <c r="D2" s="159"/>
+      <c r="E2" s="159"/>
+      <c r="F2" s="159"/>
+      <c r="G2" s="159"/>
+      <c r="H2" s="159"/>
+      <c r="I2" s="159"/>
+      <c r="J2" s="159"/>
+      <c r="K2" s="159"/>
+      <c r="L2" s="159"/>
+      <c r="M2" s="159"/>
+      <c r="N2" s="159"/>
+      <c r="O2" s="159"/>
+      <c r="P2" s="159"/>
+      <c r="Q2" s="159"/>
+      <c r="R2" s="159"/>
+      <c r="S2" s="159"/>
+      <c r="T2" s="159"/>
+      <c r="U2" s="159"/>
+      <c r="V2" s="159"/>
+      <c r="W2" s="159"/>
+      <c r="X2" s="159"/>
+      <c r="Y2" s="159"/>
+      <c r="Z2" s="159"/>
+      <c r="AA2" s="159"/>
+      <c r="AB2" s="159"/>
+      <c r="AC2" s="159"/>
+      <c r="AD2" s="159"/>
+      <c r="AE2" s="159"/>
+      <c r="AF2" s="159"/>
+      <c r="AG2" s="159"/>
+      <c r="AH2" s="159"/>
+      <c r="AI2" s="159"/>
+      <c r="AJ2" s="159"/>
+      <c r="AK2" s="159"/>
+      <c r="AL2" s="159"/>
+      <c r="AM2" s="159"/>
+      <c r="AN2" s="159"/>
+      <c r="AO2" s="159"/>
+      <c r="AP2" s="159"/>
+      <c r="AQ2" s="159"/>
+      <c r="AR2" s="159"/>
+      <c r="AS2" s="159"/>
+      <c r="AT2" s="159"/>
+      <c r="AU2" s="159"/>
+      <c r="AV2" s="159"/>
+      <c r="AW2" s="159"/>
+      <c r="AX2" s="159"/>
+      <c r="AY2" s="159"/>
+      <c r="AZ2" s="159"/>
+      <c r="BA2" s="159"/>
+      <c r="BB2" s="159"/>
       <c r="BC2" s="96"/>
       <c r="BE2" s="30"/>
     </row>
     <row r="3" spans="1:57" s="29" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="148" t="s">
+      <c r="A3" s="160" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="148"/>
-      <c r="C3" s="148"/>
-      <c r="D3" s="148"/>
-      <c r="E3" s="148"/>
-      <c r="F3" s="148"/>
-      <c r="G3" s="148"/>
-      <c r="H3" s="148"/>
-      <c r="I3" s="148"/>
-      <c r="J3" s="148"/>
-      <c r="K3" s="148"/>
-      <c r="L3" s="148"/>
-      <c r="M3" s="148"/>
-      <c r="N3" s="148"/>
-      <c r="O3" s="148"/>
-      <c r="P3" s="148"/>
-      <c r="Q3" s="148"/>
-      <c r="R3" s="148"/>
-      <c r="S3" s="148"/>
-      <c r="T3" s="148"/>
-      <c r="U3" s="148"/>
-      <c r="V3" s="148"/>
-      <c r="W3" s="148"/>
-      <c r="X3" s="148"/>
-      <c r="Y3" s="148"/>
-      <c r="Z3" s="148"/>
-      <c r="AA3" s="148"/>
-      <c r="AB3" s="148"/>
-      <c r="AC3" s="148"/>
-      <c r="AD3" s="148"/>
-      <c r="AE3" s="148"/>
-      <c r="AF3" s="148"/>
-      <c r="AG3" s="148"/>
-      <c r="AH3" s="148"/>
-      <c r="AI3" s="148"/>
-      <c r="AJ3" s="148"/>
-      <c r="AK3" s="148"/>
-      <c r="AL3" s="148"/>
-      <c r="AM3" s="148"/>
-      <c r="AN3" s="148"/>
-      <c r="AO3" s="148"/>
-      <c r="AP3" s="148"/>
-      <c r="AQ3" s="148"/>
-      <c r="AR3" s="148"/>
-      <c r="AS3" s="148"/>
-      <c r="AT3" s="148"/>
-      <c r="AU3" s="148"/>
-      <c r="AV3" s="148"/>
-      <c r="AW3" s="148"/>
-      <c r="AX3" s="148"/>
-      <c r="AY3" s="148"/>
-      <c r="AZ3" s="148"/>
-      <c r="BA3" s="148"/>
-      <c r="BB3" s="148"/>
+      <c r="B3" s="160"/>
+      <c r="C3" s="160"/>
+      <c r="D3" s="160"/>
+      <c r="E3" s="160"/>
+      <c r="F3" s="160"/>
+      <c r="G3" s="160"/>
+      <c r="H3" s="160"/>
+      <c r="I3" s="160"/>
+      <c r="J3" s="160"/>
+      <c r="K3" s="160"/>
+      <c r="L3" s="160"/>
+      <c r="M3" s="160"/>
+      <c r="N3" s="160"/>
+      <c r="O3" s="160"/>
+      <c r="P3" s="160"/>
+      <c r="Q3" s="160"/>
+      <c r="R3" s="160"/>
+      <c r="S3" s="160"/>
+      <c r="T3" s="160"/>
+      <c r="U3" s="160"/>
+      <c r="V3" s="160"/>
+      <c r="W3" s="160"/>
+      <c r="X3" s="160"/>
+      <c r="Y3" s="160"/>
+      <c r="Z3" s="160"/>
+      <c r="AA3" s="160"/>
+      <c r="AB3" s="160"/>
+      <c r="AC3" s="160"/>
+      <c r="AD3" s="160"/>
+      <c r="AE3" s="160"/>
+      <c r="AF3" s="160"/>
+      <c r="AG3" s="160"/>
+      <c r="AH3" s="160"/>
+      <c r="AI3" s="160"/>
+      <c r="AJ3" s="160"/>
+      <c r="AK3" s="160"/>
+      <c r="AL3" s="160"/>
+      <c r="AM3" s="160"/>
+      <c r="AN3" s="160"/>
+      <c r="AO3" s="160"/>
+      <c r="AP3" s="160"/>
+      <c r="AQ3" s="160"/>
+      <c r="AR3" s="160"/>
+      <c r="AS3" s="160"/>
+      <c r="AT3" s="160"/>
+      <c r="AU3" s="160"/>
+      <c r="AV3" s="160"/>
+      <c r="AW3" s="160"/>
+      <c r="AX3" s="160"/>
+      <c r="AY3" s="160"/>
+      <c r="AZ3" s="160"/>
+      <c r="BA3" s="160"/>
+      <c r="BB3" s="160"/>
       <c r="BC3" s="96"/>
       <c r="BE3" s="30"/>
     </row>
     <row r="4" spans="1:57" s="29" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="147" t="s">
+      <c r="A4" s="159" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="147"/>
-      <c r="C4" s="147"/>
-      <c r="D4" s="147"/>
-      <c r="E4" s="147"/>
-      <c r="F4" s="147"/>
-      <c r="G4" s="147"/>
-      <c r="H4" s="147"/>
-      <c r="I4" s="147"/>
-      <c r="J4" s="147"/>
-      <c r="K4" s="147"/>
-      <c r="L4" s="147"/>
-      <c r="M4" s="147"/>
-      <c r="N4" s="147"/>
-      <c r="O4" s="147"/>
-      <c r="P4" s="147"/>
-      <c r="Q4" s="147"/>
-      <c r="R4" s="147"/>
-      <c r="S4" s="147"/>
-      <c r="T4" s="147"/>
-      <c r="U4" s="147"/>
-      <c r="V4" s="147"/>
-      <c r="W4" s="147"/>
-      <c r="X4" s="147"/>
-      <c r="Y4" s="147"/>
-      <c r="Z4" s="147"/>
-      <c r="AA4" s="147"/>
-      <c r="AB4" s="147"/>
-      <c r="AC4" s="147"/>
-      <c r="AD4" s="147"/>
-      <c r="AE4" s="147"/>
-      <c r="AF4" s="147"/>
-      <c r="AG4" s="147"/>
-      <c r="AH4" s="147"/>
-      <c r="AI4" s="147"/>
-      <c r="AJ4" s="147"/>
-      <c r="AK4" s="147"/>
-      <c r="AL4" s="147"/>
-      <c r="AM4" s="147"/>
-      <c r="AN4" s="147"/>
-      <c r="AO4" s="147"/>
-      <c r="AP4" s="147"/>
-      <c r="AQ4" s="147"/>
-      <c r="AR4" s="147"/>
-      <c r="AS4" s="147"/>
-      <c r="AT4" s="147"/>
-      <c r="AU4" s="147"/>
-      <c r="AV4" s="147"/>
-      <c r="AW4" s="147"/>
-      <c r="AX4" s="147"/>
-      <c r="AY4" s="147"/>
-      <c r="AZ4" s="147"/>
-      <c r="BA4" s="147"/>
-      <c r="BB4" s="147"/>
+      <c r="B4" s="159"/>
+      <c r="C4" s="159"/>
+      <c r="D4" s="159"/>
+      <c r="E4" s="159"/>
+      <c r="F4" s="159"/>
+      <c r="G4" s="159"/>
+      <c r="H4" s="159"/>
+      <c r="I4" s="159"/>
+      <c r="J4" s="159"/>
+      <c r="K4" s="159"/>
+      <c r="L4" s="159"/>
+      <c r="M4" s="159"/>
+      <c r="N4" s="159"/>
+      <c r="O4" s="159"/>
+      <c r="P4" s="159"/>
+      <c r="Q4" s="159"/>
+      <c r="R4" s="159"/>
+      <c r="S4" s="159"/>
+      <c r="T4" s="159"/>
+      <c r="U4" s="159"/>
+      <c r="V4" s="159"/>
+      <c r="W4" s="159"/>
+      <c r="X4" s="159"/>
+      <c r="Y4" s="159"/>
+      <c r="Z4" s="159"/>
+      <c r="AA4" s="159"/>
+      <c r="AB4" s="159"/>
+      <c r="AC4" s="159"/>
+      <c r="AD4" s="159"/>
+      <c r="AE4" s="159"/>
+      <c r="AF4" s="159"/>
+      <c r="AG4" s="159"/>
+      <c r="AH4" s="159"/>
+      <c r="AI4" s="159"/>
+      <c r="AJ4" s="159"/>
+      <c r="AK4" s="159"/>
+      <c r="AL4" s="159"/>
+      <c r="AM4" s="159"/>
+      <c r="AN4" s="159"/>
+      <c r="AO4" s="159"/>
+      <c r="AP4" s="159"/>
+      <c r="AQ4" s="159"/>
+      <c r="AR4" s="159"/>
+      <c r="AS4" s="159"/>
+      <c r="AT4" s="159"/>
+      <c r="AU4" s="159"/>
+      <c r="AV4" s="159"/>
+      <c r="AW4" s="159"/>
+      <c r="AX4" s="159"/>
+      <c r="AY4" s="159"/>
+      <c r="AZ4" s="159"/>
+      <c r="BA4" s="159"/>
+      <c r="BB4" s="159"/>
       <c r="BC4" s="96"/>
       <c r="BE4" s="30"/>
     </row>
     <row r="5" spans="1:57" s="29" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="149" t="s">
+      <c r="A5" s="161" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="149"/>
-      <c r="C5" s="149"/>
-      <c r="D5" s="149"/>
-      <c r="E5" s="149"/>
-      <c r="F5" s="149"/>
-      <c r="G5" s="149"/>
-      <c r="H5" s="149"/>
-      <c r="I5" s="149"/>
-      <c r="J5" s="149"/>
-      <c r="K5" s="149"/>
-      <c r="L5" s="149"/>
-      <c r="M5" s="149"/>
-      <c r="N5" s="149"/>
-      <c r="O5" s="149"/>
-      <c r="P5" s="149"/>
-      <c r="Q5" s="149"/>
-      <c r="R5" s="149"/>
-      <c r="S5" s="149"/>
-      <c r="T5" s="149"/>
-      <c r="U5" s="149"/>
-      <c r="V5" s="149"/>
-      <c r="W5" s="149"/>
-      <c r="X5" s="149"/>
-      <c r="Y5" s="149"/>
-      <c r="Z5" s="149"/>
-      <c r="AA5" s="149"/>
-      <c r="AB5" s="149"/>
-      <c r="AC5" s="149"/>
-      <c r="AD5" s="149"/>
-      <c r="AE5" s="149"/>
-      <c r="AF5" s="149"/>
-      <c r="AG5" s="149"/>
-      <c r="AH5" s="149"/>
-      <c r="AI5" s="149"/>
-      <c r="AJ5" s="149"/>
-      <c r="AK5" s="149"/>
-      <c r="AL5" s="149"/>
-      <c r="AM5" s="149"/>
-      <c r="AN5" s="149"/>
-      <c r="AO5" s="149"/>
-      <c r="AP5" s="149"/>
-      <c r="AQ5" s="149"/>
-      <c r="AR5" s="149"/>
-      <c r="AS5" s="149"/>
-      <c r="AT5" s="149"/>
-      <c r="AU5" s="149"/>
-      <c r="AV5" s="149"/>
-      <c r="AW5" s="149"/>
-      <c r="AX5" s="149"/>
-      <c r="AY5" s="149"/>
-      <c r="AZ5" s="149"/>
-      <c r="BA5" s="149"/>
-      <c r="BB5" s="149"/>
+      <c r="B5" s="161"/>
+      <c r="C5" s="161"/>
+      <c r="D5" s="161"/>
+      <c r="E5" s="161"/>
+      <c r="F5" s="161"/>
+      <c r="G5" s="161"/>
+      <c r="H5" s="161"/>
+      <c r="I5" s="161"/>
+      <c r="J5" s="161"/>
+      <c r="K5" s="161"/>
+      <c r="L5" s="161"/>
+      <c r="M5" s="161"/>
+      <c r="N5" s="161"/>
+      <c r="O5" s="161"/>
+      <c r="P5" s="161"/>
+      <c r="Q5" s="161"/>
+      <c r="R5" s="161"/>
+      <c r="S5" s="161"/>
+      <c r="T5" s="161"/>
+      <c r="U5" s="161"/>
+      <c r="V5" s="161"/>
+      <c r="W5" s="161"/>
+      <c r="X5" s="161"/>
+      <c r="Y5" s="161"/>
+      <c r="Z5" s="161"/>
+      <c r="AA5" s="161"/>
+      <c r="AB5" s="161"/>
+      <c r="AC5" s="161"/>
+      <c r="AD5" s="161"/>
+      <c r="AE5" s="161"/>
+      <c r="AF5" s="161"/>
+      <c r="AG5" s="161"/>
+      <c r="AH5" s="161"/>
+      <c r="AI5" s="161"/>
+      <c r="AJ5" s="161"/>
+      <c r="AK5" s="161"/>
+      <c r="AL5" s="161"/>
+      <c r="AM5" s="161"/>
+      <c r="AN5" s="161"/>
+      <c r="AO5" s="161"/>
+      <c r="AP5" s="161"/>
+      <c r="AQ5" s="161"/>
+      <c r="AR5" s="161"/>
+      <c r="AS5" s="161"/>
+      <c r="AT5" s="161"/>
+      <c r="AU5" s="161"/>
+      <c r="AV5" s="161"/>
+      <c r="AW5" s="161"/>
+      <c r="AX5" s="161"/>
+      <c r="AY5" s="161"/>
+      <c r="AZ5" s="161"/>
+      <c r="BA5" s="161"/>
+      <c r="BB5" s="161"/>
       <c r="BC5" s="96"/>
       <c r="BE5" s="30"/>
     </row>
@@ -5326,94 +5326,94 @@
       <c r="BE6" s="30"/>
     </row>
     <row r="7" spans="1:57" s="29" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="169" t="s">
+      <c r="A7" s="171" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="170"/>
-      <c r="C7" s="164" t="s">
+      <c r="B7" s="172"/>
+      <c r="C7" s="166" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="165"/>
-      <c r="E7" s="165"/>
-      <c r="F7" s="165"/>
-      <c r="G7" s="164" t="s">
+      <c r="D7" s="167"/>
+      <c r="E7" s="167"/>
+      <c r="F7" s="167"/>
+      <c r="G7" s="166" t="s">
         <v>64</v>
       </c>
-      <c r="H7" s="165"/>
-      <c r="I7" s="165"/>
-      <c r="J7" s="166"/>
-      <c r="K7" s="165" t="s">
+      <c r="H7" s="167"/>
+      <c r="I7" s="167"/>
+      <c r="J7" s="168"/>
+      <c r="K7" s="167" t="s">
         <v>65</v>
       </c>
-      <c r="L7" s="165"/>
-      <c r="M7" s="165"/>
-      <c r="N7" s="165"/>
-      <c r="O7" s="165"/>
-      <c r="P7" s="164" t="s">
+      <c r="L7" s="167"/>
+      <c r="M7" s="167"/>
+      <c r="N7" s="167"/>
+      <c r="O7" s="167"/>
+      <c r="P7" s="166" t="s">
         <v>66</v>
       </c>
-      <c r="Q7" s="165"/>
-      <c r="R7" s="165"/>
-      <c r="S7" s="165"/>
-      <c r="T7" s="166"/>
-      <c r="U7" s="164" t="s">
+      <c r="Q7" s="167"/>
+      <c r="R7" s="167"/>
+      <c r="S7" s="167"/>
+      <c r="T7" s="168"/>
+      <c r="U7" s="166" t="s">
         <v>55</v>
       </c>
-      <c r="V7" s="165"/>
-      <c r="W7" s="165"/>
-      <c r="X7" s="165"/>
-      <c r="Y7" s="165"/>
-      <c r="Z7" s="164" t="s">
+      <c r="V7" s="167"/>
+      <c r="W7" s="167"/>
+      <c r="X7" s="167"/>
+      <c r="Y7" s="167"/>
+      <c r="Z7" s="166" t="s">
         <v>56</v>
       </c>
-      <c r="AA7" s="165"/>
-      <c r="AB7" s="165"/>
-      <c r="AC7" s="166"/>
-      <c r="AD7" s="164" t="s">
+      <c r="AA7" s="167"/>
+      <c r="AB7" s="167"/>
+      <c r="AC7" s="168"/>
+      <c r="AD7" s="166" t="s">
         <v>57</v>
       </c>
-      <c r="AE7" s="165"/>
-      <c r="AF7" s="165"/>
-      <c r="AG7" s="166"/>
-      <c r="AH7" s="164" t="s">
+      <c r="AE7" s="167"/>
+      <c r="AF7" s="167"/>
+      <c r="AG7" s="168"/>
+      <c r="AH7" s="166" t="s">
         <v>58</v>
       </c>
-      <c r="AI7" s="165"/>
-      <c r="AJ7" s="165"/>
-      <c r="AK7" s="166"/>
-      <c r="AL7" s="165" t="s">
+      <c r="AI7" s="167"/>
+      <c r="AJ7" s="167"/>
+      <c r="AK7" s="168"/>
+      <c r="AL7" s="167" t="s">
         <v>59</v>
       </c>
-      <c r="AM7" s="165"/>
-      <c r="AN7" s="165"/>
-      <c r="AO7" s="166"/>
-      <c r="AP7" s="164" t="s">
+      <c r="AM7" s="167"/>
+      <c r="AN7" s="167"/>
+      <c r="AO7" s="168"/>
+      <c r="AP7" s="166" t="s">
         <v>60</v>
       </c>
-      <c r="AQ7" s="165"/>
-      <c r="AR7" s="165"/>
-      <c r="AS7" s="166"/>
-      <c r="AT7" s="164" t="s">
+      <c r="AQ7" s="167"/>
+      <c r="AR7" s="167"/>
+      <c r="AS7" s="168"/>
+      <c r="AT7" s="166" t="s">
         <v>61</v>
       </c>
-      <c r="AU7" s="165"/>
-      <c r="AV7" s="165"/>
-      <c r="AW7" s="166"/>
-      <c r="AX7" s="164" t="s">
+      <c r="AU7" s="167"/>
+      <c r="AV7" s="167"/>
+      <c r="AW7" s="168"/>
+      <c r="AX7" s="166" t="s">
         <v>62</v>
       </c>
-      <c r="AY7" s="165"/>
-      <c r="AZ7" s="165"/>
-      <c r="BA7" s="165"/>
-      <c r="BB7" s="166"/>
-      <c r="BC7" s="175" t="s">
+      <c r="AY7" s="167"/>
+      <c r="AZ7" s="167"/>
+      <c r="BA7" s="167"/>
+      <c r="BB7" s="168"/>
+      <c r="BC7" s="164" t="s">
         <v>96</v>
       </c>
       <c r="BE7" s="30"/>
     </row>
     <row r="8" spans="1:57" s="29" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="171"/>
-      <c r="B8" s="172"/>
+      <c r="A8" s="173"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="33"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
@@ -5466,14 +5466,14 @@
       <c r="AZ8" s="35"/>
       <c r="BA8" s="35"/>
       <c r="BB8" s="134"/>
-      <c r="BC8" s="176"/>
+      <c r="BC8" s="165"/>
       <c r="BE8" s="30"/>
     </row>
     <row r="9" spans="1:57" s="29" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="175" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="176"/>
       <c r="C9" s="133" t="s">
         <v>24</v>
       </c>
@@ -5630,7 +5630,7 @@
       <c r="BB9" s="131" t="s">
         <v>94</v>
       </c>
-      <c r="BC9" s="176"/>
+      <c r="BC9" s="165"/>
       <c r="BE9" s="30"/>
     </row>
     <row r="10" spans="1:57" s="29" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7679,10 +7679,10 @@
       <c r="BE34" s="30"/>
     </row>
     <row r="35" spans="1:57" s="29" customFormat="1" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="167" t="s">
+      <c r="A35" s="169" t="s">
         <v>95</v>
       </c>
-      <c r="B35" s="168"/>
+      <c r="B35" s="170"/>
       <c r="C35" s="101">
         <f t="shared" ref="C35:AH35" si="1">SUM(C10:C34)</f>
         <v>11</v>
@@ -8007,11 +8007,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="BC7:BC9"/>
-    <mergeCell ref="AT7:AW7"/>
-    <mergeCell ref="AP7:AS7"/>
-    <mergeCell ref="AL7:AO7"/>
-    <mergeCell ref="AH7:AK7"/>
+    <mergeCell ref="A1:BB1"/>
+    <mergeCell ref="A2:BB2"/>
+    <mergeCell ref="A3:BB3"/>
+    <mergeCell ref="A4:BB4"/>
+    <mergeCell ref="A5:BB5"/>
     <mergeCell ref="AD7:AG7"/>
     <mergeCell ref="AX7:BB7"/>
     <mergeCell ref="A35:B35"/>
@@ -8023,14 +8023,14 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="U7:Y7"/>
     <mergeCell ref="Z7:AC7"/>
-    <mergeCell ref="A1:BB1"/>
-    <mergeCell ref="A2:BB2"/>
-    <mergeCell ref="A3:BB3"/>
-    <mergeCell ref="A4:BB4"/>
-    <mergeCell ref="A5:BB5"/>
+    <mergeCell ref="BC7:BC9"/>
+    <mergeCell ref="AT7:AW7"/>
+    <mergeCell ref="AP7:AS7"/>
+    <mergeCell ref="AL7:AO7"/>
+    <mergeCell ref="AH7:AK7"/>
   </mergeCells>
   <pageMargins left="0.25" right="1.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" scale="53" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="5" scale="54" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>